<commit_message>
Switched to original data file
</commit_message>
<xml_diff>
--- a/DataFile.xlsx
+++ b/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E60E00-4AC9-4D33-9AE2-63CC2F9303CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B328F1F-13A0-464B-8811-09CCCC941A19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="3705" windowWidth="21600" windowHeight="10290" activeTab="4" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
@@ -2757,8 +2757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F027EA97-39C6-4A00-847A-7E78910072DF}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4229,7 +4229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C30AA8-3415-4BDB-A606-A9FA09E8CC8D}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fixes with the number 2
</commit_message>
<xml_diff>
--- a/DataFile.xlsx
+++ b/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chakotay Incorvaia\dev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\ICT3911Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A08FDD6-2ED3-4795-803E-0E885C95A2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A15BF8-AEE3-4578-BEDB-1E59E735FC37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCE0E44F-0ABA-4097-A493-E6A10D57D926}"/>
   </bookViews>
   <sheets>
     <sheet name="QualitySheet" sheetId="1" r:id="rId1"/>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A2CE25-1FB0-46F3-A95B-A7BCC2B1E34D}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B39" sqref="B38:B39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2023,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>